<commit_message>
wrote test for getWorkSheetData()
</commit_message>
<xml_diff>
--- a/doc-file.xlsx
+++ b/doc-file.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Tabelle1" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="TestSheet" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="R1C1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="110">
   <si>
     <t xml:space="preserve">Basic flow</t>
   </si>
@@ -264,6 +265,93 @@
   </si>
   <si>
     <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scoring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aaaaaaaaaa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aaaaaaaaab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inconsistent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aaaaaaaabc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aaaaaaabcd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aaaaaabcde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aaaaabcdef</t>
+  </si>
+  <si>
+    <t xml:space="preserve">missing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aaaabcdefg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aaabcdefgh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aabcdefghi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abcdefghij</t>
+  </si>
+  <si>
+    <t xml:space="preserve">position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pos1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$and</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$or</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aa,bb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ee,ff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ff</t>
   </si>
 </sst>
 </file>
@@ -275,7 +363,7 @@
     <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="&quot;WAHR&quot;;&quot;WAHR&quot;;&quot;FALSCH&quot;"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -325,6 +413,34 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF996600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -358,7 +474,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -370,6 +486,34 @@
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
@@ -408,7 +552,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -491,6 +635,54 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -681,7 +873,7 @@
   </sheetPr>
   <dimension ref="A2:K76"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1342,7 +1534,7 @@
   </sheetPr>
   <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M6" activeCellId="0" sqref="M6"/>
     </sheetView>
   </sheetViews>
@@ -2571,4 +2763,397 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B1:J42"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B2" s="21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="23" t="n">
+        <v>2.22044604925031E-016</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B5" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="24" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B6" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="24" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="24" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="24" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B9" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="25" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B10" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="25" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" s="25" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="25" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B13" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="25" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="F18" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="G18" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="E19" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="F19" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="G19" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="H19" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B20" s="26"/>
+      <c r="C20" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="D20" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="E20" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="H20" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="I20" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="J20" s="26"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B21" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="C21" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="D21" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="E21" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="G21" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="I21" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="J21" s="27" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B22" s="26"/>
+      <c r="C22" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="D22" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="E22" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="F22" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="H22" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="I22" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="J22" s="26"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="E23" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="F23" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="G23" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="H23" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="F24" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="G24" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B27" s="21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B29" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="F29" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="G29" s="21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E30" s="21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B31" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C31" s="30"/>
+      <c r="E31" s="21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E32" s="21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B33" s="29"/>
+      <c r="C33" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="E33" s="21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E34" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B35" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="E35" s="21" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B36" s="32" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B38" s="31" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B39" s="32"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B41" s="31"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B42" s="32" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>